<commit_message>
resumo BERTopic e alguns tweets
</commit_message>
<xml_diff>
--- a/State of Art/Article KeyWords.xlsx
+++ b/State of Art/Article KeyWords.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\claud\OneDrive\Ambiente de Trabalho\Tese\State of Art\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\claud\OneDrive\Ambiente de Trabalho\tese\State of Art\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B143281C-5E2C-40B6-ACC6-FE37ABA30268}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFA6DEF9-E4FC-4A9B-B035-A803F97BADE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{A4B60097-D1DB-47A4-812B-C06D94CFCCF5}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="32">
   <si>
     <t>Article</t>
   </si>
@@ -129,6 +129,9 @@
   </si>
   <si>
     <t>Nº Resumo</t>
+  </si>
+  <si>
+    <t>BERTopic, c-TFIDF, MiniLM, HDBSCAN</t>
   </si>
 </sst>
 </file>
@@ -246,7 +249,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -299,6 +302,9 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -638,7 +644,7 @@
   <dimension ref="A1:E100"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -674,12 +680,14 @@
       <c r="B2" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="10" t="s">
+      <c r="C2" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="4" t="s">
-        <v>7</v>
+      <c r="E2" s="4">
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
@@ -1633,6 +1641,7 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D10" r:id="rId1" xr:uid="{4A391570-ABC8-4EA9-AC37-6BDF51810E72}"/>
+    <hyperlink ref="D2" r:id="rId2" xr:uid="{91F9D23D-409C-4290-AA4F-1D3BC4883956}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
inicial analysis and 330
</commit_message>
<xml_diff>
--- a/State of Art/Article KeyWords.xlsx
+++ b/State of Art/Article KeyWords.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\claud\OneDrive\Ambiente de Trabalho\tese\State of Art\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93148F8E-DAE5-40D7-826A-289F2875D70E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51A734FF-0E7A-4862-8FBA-6F922571681F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{A4B60097-D1DB-47A4-812B-C06D94CFCCF5}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="39">
   <si>
     <t>Article</t>
   </si>
@@ -141,6 +141,18 @@
   </si>
   <si>
     <t>Change in large networks, Clustering, Bootstrap, Alluvial diagram</t>
+  </si>
+  <si>
+    <t>Topic Mining, BERTopic, 117th Congress, Twitter, short-text data</t>
+  </si>
+  <si>
+    <t>Latent Dirichlet Allocation (LDA), Dynamic Topic Models (DTM)</t>
+  </si>
+  <si>
+    <t>Graphical Models, Temporal Analysis, Topic Modeling</t>
+  </si>
+  <si>
+    <t>Clustering, Hierarchical model, Markov chain Monte Carlo, Mixture model, Nonparametric Bayesian statistics</t>
   </si>
 </sst>
 </file>
@@ -264,7 +276,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -326,6 +338,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -670,7 +685,7 @@
   <dimension ref="A1:E100"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -774,12 +789,14 @@
       <c r="B6" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="3"/>
-      <c r="D6" s="10" t="s">
+      <c r="C6" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D6" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="E6" s="21" t="s">
-        <v>7</v>
+      <c r="E6" s="4">
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
@@ -789,12 +806,14 @@
       <c r="B7" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="3"/>
-      <c r="D7" s="10" t="s">
+      <c r="C7" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D7" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="E7" s="21" t="s">
-        <v>7</v>
+      <c r="E7" s="4">
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
@@ -804,11 +823,13 @@
       <c r="B8" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="3"/>
-      <c r="D8" s="9" t="s">
+      <c r="C8" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D8" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="E8" s="21" t="s">
+      <c r="E8" s="4">
         <v>7</v>
       </c>
     </row>
@@ -819,12 +840,14 @@
       <c r="B9" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="3"/>
-      <c r="D9" s="9" t="s">
+      <c r="C9" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="D9" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="E9" s="21" t="s">
-        <v>7</v>
+      <c r="E9" s="4">
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
@@ -1677,6 +1700,10 @@
     <hyperlink ref="D3" r:id="rId3" xr:uid="{76047C10-54C9-4093-ADAB-3879E27C8ED4}"/>
     <hyperlink ref="D4" r:id="rId4" xr:uid="{F0577C92-3F54-4FD5-892B-158F2A6A04F6}"/>
     <hyperlink ref="D5" r:id="rId5" xr:uid="{B6A1D46F-B609-494A-812E-B6E5A43CE0C2}"/>
+    <hyperlink ref="D6" r:id="rId6" xr:uid="{2ED2058A-EABB-43FF-8A3C-82A9097BCA0A}"/>
+    <hyperlink ref="D7" r:id="rId7" xr:uid="{8202EC2E-9625-4D49-89C7-51A19332FAD6}"/>
+    <hyperlink ref="D8" r:id="rId8" xr:uid="{919A6496-BDCE-403C-BF9C-0D85A8386AFD}"/>
+    <hyperlink ref="D9" r:id="rId9" xr:uid="{3E263C84-41E4-4843-8811-3A6C45C9899D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
end of tweet per member and creation of week slices and the big dataset with all the info
</commit_message>
<xml_diff>
--- a/State of Art/Article KeyWords.xlsx
+++ b/State of Art/Article KeyWords.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\claud\OneDrive\Ambiente de Trabalho\tese\State of Art\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51A734FF-0E7A-4862-8FBA-6F922571681F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5014DC41-4D9E-4237-8255-447E735A8961}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{A4B60097-D1DB-47A4-812B-C06D94CFCCF5}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="40">
   <si>
     <t>Article</t>
   </si>
@@ -153,6 +153,9 @@
   </si>
   <si>
     <t>Clustering, Hierarchical model, Markov chain Monte Carlo, Mixture model, Nonparametric Bayesian statistics</t>
+  </si>
+  <si>
+    <t>Clustering, Temporal Evolution, Agglomerative, k-means, Online</t>
   </si>
 </sst>
 </file>
@@ -685,7 +688,7 @@
   <dimension ref="A1:E100"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -857,12 +860,14 @@
       <c r="B10" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C10" s="3"/>
+      <c r="C10" s="3" t="s">
+        <v>39</v>
+      </c>
       <c r="D10" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="E10" s="21" t="s">
-        <v>7</v>
+      <c r="E10" s="4">
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
visualizations and uogrades in functions
</commit_message>
<xml_diff>
--- a/State of Art/Article KeyWords.xlsx
+++ b/State of Art/Article KeyWords.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\claud\OneDrive\Ambiente de Trabalho\tese\State of Art\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89AF7DC4-8531-42F2-9DA5-C8D6956CE0C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2841873-4B96-40B4-86FD-14A775DAD799}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{A4B60097-D1DB-47A4-812B-C06D94CFCCF5}"/>
   </bookViews>
@@ -162,7 +162,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -188,12 +188,6 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -279,7 +273,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -312,25 +306,22 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -688,7 +679,7 @@
   <dimension ref="A1:E100"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -700,20 +691,20 @@
     <col min="5" max="5" width="11.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="13" customFormat="1" ht="22.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+    <row r="1" spans="1:5" s="12" customFormat="1" ht="22.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="C1" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="17" t="s">
+      <c r="D1" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="18" t="s">
+      <c r="E1" s="17" t="s">
         <v>30</v>
       </c>
     </row>
@@ -727,7 +718,7 @@
       <c r="C2" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="D2" s="19" t="s">
+      <c r="D2" s="18" t="s">
         <v>6</v>
       </c>
       <c r="E2" s="4">
@@ -744,7 +735,7 @@
       <c r="C3" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D3" s="19" t="s">
+      <c r="D3" s="18" t="s">
         <v>12</v>
       </c>
       <c r="E3" s="4">
@@ -758,10 +749,10 @@
       <c r="B4" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="20" t="s">
+      <c r="C4" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="D4" s="19" t="s">
+      <c r="D4" s="18" t="s">
         <v>13</v>
       </c>
       <c r="E4" s="4">
@@ -778,7 +769,7 @@
       <c r="C5" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="D5" s="19" t="s">
+      <c r="D5" s="18" t="s">
         <v>14</v>
       </c>
       <c r="E5" s="4">
@@ -795,7 +786,7 @@
       <c r="C6" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="D6" s="19" t="s">
+      <c r="D6" s="18" t="s">
         <v>15</v>
       </c>
       <c r="E6" s="4">
@@ -812,7 +803,7 @@
       <c r="C7" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D7" s="19" t="s">
+      <c r="D7" s="18" t="s">
         <v>23</v>
       </c>
       <c r="E7" s="4">
@@ -829,7 +820,7 @@
       <c r="C8" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="D8" s="22" t="s">
+      <c r="D8" s="21" t="s">
         <v>24</v>
       </c>
       <c r="E8" s="4">
@@ -843,10 +834,10 @@
       <c r="B9" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="20" t="s">
+      <c r="C9" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="D9" s="22" t="s">
+      <c r="D9" s="21" t="s">
         <v>25</v>
       </c>
       <c r="E9" s="4">
@@ -860,10 +851,10 @@
       <c r="B10" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C10" s="20" t="s">
+      <c r="C10" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="D10" s="12" t="s">
+      <c r="D10" s="18" t="s">
         <v>26</v>
       </c>
       <c r="E10" s="4">
@@ -881,7 +872,7 @@
       <c r="D11" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="E11" s="21" t="s">
+      <c r="E11" s="20" t="s">
         <v>7</v>
       </c>
     </row>
@@ -896,7 +887,7 @@
       <c r="D12" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="E12" s="21" t="s">
+      <c r="E12" s="20" t="s">
         <v>7</v>
       </c>
     </row>
@@ -911,7 +902,7 @@
       <c r="D13" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="E13" s="21" t="s">
+      <c r="E13" s="20" t="s">
         <v>7</v>
       </c>
     </row>
@@ -920,7 +911,7 @@
       <c r="B14" s="2"/>
       <c r="C14" s="3"/>
       <c r="D14" s="10"/>
-      <c r="E14" s="21" t="s">
+      <c r="E14" s="20" t="s">
         <v>7</v>
       </c>
     </row>
@@ -929,7 +920,7 @@
       <c r="B15" s="2"/>
       <c r="C15" s="3"/>
       <c r="D15" s="10"/>
-      <c r="E15" s="21" t="s">
+      <c r="E15" s="20" t="s">
         <v>7</v>
       </c>
     </row>
@@ -938,7 +929,7 @@
       <c r="B16" s="2"/>
       <c r="C16" s="3"/>
       <c r="D16" s="10"/>
-      <c r="E16" s="21" t="s">
+      <c r="E16" s="20" t="s">
         <v>7</v>
       </c>
     </row>
@@ -947,7 +938,7 @@
       <c r="B17" s="2"/>
       <c r="C17" s="3"/>
       <c r="D17" s="10"/>
-      <c r="E17" s="21" t="s">
+      <c r="E17" s="20" t="s">
         <v>7</v>
       </c>
     </row>
@@ -956,7 +947,7 @@
       <c r="B18" s="2"/>
       <c r="C18" s="3"/>
       <c r="D18" s="10"/>
-      <c r="E18" s="21" t="s">
+      <c r="E18" s="20" t="s">
         <v>7</v>
       </c>
     </row>
@@ -965,7 +956,7 @@
       <c r="B19" s="2"/>
       <c r="C19" s="3"/>
       <c r="D19" s="10"/>
-      <c r="E19" s="21" t="s">
+      <c r="E19" s="20" t="s">
         <v>7</v>
       </c>
     </row>
@@ -974,7 +965,7 @@
       <c r="B20" s="2"/>
       <c r="C20" s="3"/>
       <c r="D20" s="10"/>
-      <c r="E20" s="21" t="s">
+      <c r="E20" s="20" t="s">
         <v>7</v>
       </c>
     </row>
@@ -983,7 +974,7 @@
       <c r="B21" s="2"/>
       <c r="C21" s="3"/>
       <c r="D21" s="10"/>
-      <c r="E21" s="21" t="s">
+      <c r="E21" s="20" t="s">
         <v>7</v>
       </c>
     </row>
@@ -992,7 +983,7 @@
       <c r="B22" s="2"/>
       <c r="C22" s="3"/>
       <c r="D22" s="10"/>
-      <c r="E22" s="21" t="s">
+      <c r="E22" s="20" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1001,7 +992,7 @@
       <c r="B23" s="2"/>
       <c r="C23" s="3"/>
       <c r="D23" s="10"/>
-      <c r="E23" s="21" t="s">
+      <c r="E23" s="20" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1010,7 +1001,7 @@
       <c r="B24" s="2"/>
       <c r="C24" s="3"/>
       <c r="D24" s="10"/>
-      <c r="E24" s="21" t="s">
+      <c r="E24" s="20" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1019,7 +1010,7 @@
       <c r="B25" s="2"/>
       <c r="C25" s="3"/>
       <c r="D25" s="10"/>
-      <c r="E25" s="21" t="s">
+      <c r="E25" s="20" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1028,7 +1019,7 @@
       <c r="B26" s="2"/>
       <c r="C26" s="3"/>
       <c r="D26" s="10"/>
-      <c r="E26" s="21" t="s">
+      <c r="E26" s="20" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1037,7 +1028,7 @@
       <c r="B27" s="2"/>
       <c r="C27" s="3"/>
       <c r="D27" s="10"/>
-      <c r="E27" s="21" t="s">
+      <c r="E27" s="20" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1046,7 +1037,7 @@
       <c r="B28" s="2"/>
       <c r="C28" s="3"/>
       <c r="D28" s="10"/>
-      <c r="E28" s="21" t="s">
+      <c r="E28" s="20" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1055,7 +1046,7 @@
       <c r="B29" s="2"/>
       <c r="C29" s="3"/>
       <c r="D29" s="10"/>
-      <c r="E29" s="21" t="s">
+      <c r="E29" s="20" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1064,7 +1055,7 @@
       <c r="B30" s="2"/>
       <c r="C30" s="3"/>
       <c r="D30" s="10"/>
-      <c r="E30" s="21" t="s">
+      <c r="E30" s="20" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1073,7 +1064,7 @@
       <c r="B31" s="2"/>
       <c r="C31" s="3"/>
       <c r="D31" s="10"/>
-      <c r="E31" s="21" t="s">
+      <c r="E31" s="20" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1082,7 +1073,7 @@
       <c r="B32" s="2"/>
       <c r="C32" s="3"/>
       <c r="D32" s="10"/>
-      <c r="E32" s="21" t="s">
+      <c r="E32" s="20" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1091,7 +1082,7 @@
       <c r="B33" s="2"/>
       <c r="C33" s="3"/>
       <c r="D33" s="10"/>
-      <c r="E33" s="21" t="s">
+      <c r="E33" s="20" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1100,7 +1091,7 @@
       <c r="B34" s="2"/>
       <c r="C34" s="3"/>
       <c r="D34" s="10"/>
-      <c r="E34" s="21" t="s">
+      <c r="E34" s="20" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1109,7 +1100,7 @@
       <c r="B35" s="2"/>
       <c r="C35" s="3"/>
       <c r="D35" s="10"/>
-      <c r="E35" s="21" t="s">
+      <c r="E35" s="20" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1118,7 +1109,7 @@
       <c r="B36" s="2"/>
       <c r="C36" s="3"/>
       <c r="D36" s="10"/>
-      <c r="E36" s="21" t="s">
+      <c r="E36" s="20" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1127,7 +1118,7 @@
       <c r="B37" s="2"/>
       <c r="C37" s="3"/>
       <c r="D37" s="10"/>
-      <c r="E37" s="21" t="s">
+      <c r="E37" s="20" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1136,7 +1127,7 @@
       <c r="B38" s="2"/>
       <c r="C38" s="3"/>
       <c r="D38" s="10"/>
-      <c r="E38" s="21" t="s">
+      <c r="E38" s="20" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1145,7 +1136,7 @@
       <c r="B39" s="2"/>
       <c r="C39" s="3"/>
       <c r="D39" s="10"/>
-      <c r="E39" s="21" t="s">
+      <c r="E39" s="20" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1154,7 +1145,7 @@
       <c r="B40" s="2"/>
       <c r="C40" s="3"/>
       <c r="D40" s="10"/>
-      <c r="E40" s="21" t="s">
+      <c r="E40" s="20" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1163,7 +1154,7 @@
       <c r="B41" s="2"/>
       <c r="C41" s="3"/>
       <c r="D41" s="10"/>
-      <c r="E41" s="21" t="s">
+      <c r="E41" s="20" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1172,7 +1163,7 @@
       <c r="B42" s="2"/>
       <c r="C42" s="3"/>
       <c r="D42" s="10"/>
-      <c r="E42" s="21" t="s">
+      <c r="E42" s="20" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1181,7 +1172,7 @@
       <c r="B43" s="2"/>
       <c r="C43" s="3"/>
       <c r="D43" s="10"/>
-      <c r="E43" s="21" t="s">
+      <c r="E43" s="20" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1190,7 +1181,7 @@
       <c r="B44" s="2"/>
       <c r="C44" s="3"/>
       <c r="D44" s="10"/>
-      <c r="E44" s="21" t="s">
+      <c r="E44" s="20" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1199,7 +1190,7 @@
       <c r="B45" s="2"/>
       <c r="C45" s="3"/>
       <c r="D45" s="10"/>
-      <c r="E45" s="21" t="s">
+      <c r="E45" s="20" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1208,7 +1199,7 @@
       <c r="B46" s="2"/>
       <c r="C46" s="3"/>
       <c r="D46" s="10"/>
-      <c r="E46" s="21" t="s">
+      <c r="E46" s="20" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1217,7 +1208,7 @@
       <c r="B47" s="2"/>
       <c r="C47" s="3"/>
       <c r="D47" s="10"/>
-      <c r="E47" s="21" t="s">
+      <c r="E47" s="20" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1226,7 +1217,7 @@
       <c r="B48" s="2"/>
       <c r="C48" s="3"/>
       <c r="D48" s="10"/>
-      <c r="E48" s="21" t="s">
+      <c r="E48" s="20" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1235,7 +1226,7 @@
       <c r="B49" s="2"/>
       <c r="C49" s="3"/>
       <c r="D49" s="10"/>
-      <c r="E49" s="21" t="s">
+      <c r="E49" s="20" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1244,7 +1235,7 @@
       <c r="B50" s="2"/>
       <c r="C50" s="3"/>
       <c r="D50" s="10"/>
-      <c r="E50" s="21" t="s">
+      <c r="E50" s="20" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1253,7 +1244,7 @@
       <c r="B51" s="2"/>
       <c r="C51" s="3"/>
       <c r="D51" s="10"/>
-      <c r="E51" s="21" t="s">
+      <c r="E51" s="20" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1262,7 +1253,7 @@
       <c r="B52" s="2"/>
       <c r="C52" s="3"/>
       <c r="D52" s="10"/>
-      <c r="E52" s="21" t="s">
+      <c r="E52" s="20" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1271,7 +1262,7 @@
       <c r="B53" s="2"/>
       <c r="C53" s="3"/>
       <c r="D53" s="10"/>
-      <c r="E53" s="21" t="s">
+      <c r="E53" s="20" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1280,7 +1271,7 @@
       <c r="B54" s="2"/>
       <c r="C54" s="3"/>
       <c r="D54" s="10"/>
-      <c r="E54" s="21" t="s">
+      <c r="E54" s="20" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1289,7 +1280,7 @@
       <c r="B55" s="2"/>
       <c r="C55" s="3"/>
       <c r="D55" s="10"/>
-      <c r="E55" s="21" t="s">
+      <c r="E55" s="20" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1298,7 +1289,7 @@
       <c r="B56" s="2"/>
       <c r="C56" s="3"/>
       <c r="D56" s="10"/>
-      <c r="E56" s="21" t="s">
+      <c r="E56" s="20" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1307,7 +1298,7 @@
       <c r="B57" s="2"/>
       <c r="C57" s="3"/>
       <c r="D57" s="10"/>
-      <c r="E57" s="21" t="s">
+      <c r="E57" s="20" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1316,7 +1307,7 @@
       <c r="B58" s="2"/>
       <c r="C58" s="3"/>
       <c r="D58" s="10"/>
-      <c r="E58" s="21" t="s">
+      <c r="E58" s="20" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1325,7 +1316,7 @@
       <c r="B59" s="2"/>
       <c r="C59" s="3"/>
       <c r="D59" s="10"/>
-      <c r="E59" s="21" t="s">
+      <c r="E59" s="20" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1334,7 +1325,7 @@
       <c r="B60" s="2"/>
       <c r="C60" s="3"/>
       <c r="D60" s="10"/>
-      <c r="E60" s="21" t="s">
+      <c r="E60" s="20" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1343,7 +1334,7 @@
       <c r="B61" s="2"/>
       <c r="C61" s="3"/>
       <c r="D61" s="10"/>
-      <c r="E61" s="21" t="s">
+      <c r="E61" s="20" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1352,7 +1343,7 @@
       <c r="B62" s="2"/>
       <c r="C62" s="3"/>
       <c r="D62" s="10"/>
-      <c r="E62" s="21" t="s">
+      <c r="E62" s="20" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1361,7 +1352,7 @@
       <c r="B63" s="2"/>
       <c r="C63" s="3"/>
       <c r="D63" s="10"/>
-      <c r="E63" s="21" t="s">
+      <c r="E63" s="20" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1370,7 +1361,7 @@
       <c r="B64" s="2"/>
       <c r="C64" s="3"/>
       <c r="D64" s="10"/>
-      <c r="E64" s="21" t="s">
+      <c r="E64" s="20" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1379,7 +1370,7 @@
       <c r="B65" s="2"/>
       <c r="C65" s="3"/>
       <c r="D65" s="10"/>
-      <c r="E65" s="21" t="s">
+      <c r="E65" s="20" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1388,7 +1379,7 @@
       <c r="B66" s="2"/>
       <c r="C66" s="3"/>
       <c r="D66" s="10"/>
-      <c r="E66" s="21" t="s">
+      <c r="E66" s="20" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1397,7 +1388,7 @@
       <c r="B67" s="2"/>
       <c r="C67" s="3"/>
       <c r="D67" s="10"/>
-      <c r="E67" s="21" t="s">
+      <c r="E67" s="20" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1406,7 +1397,7 @@
       <c r="B68" s="2"/>
       <c r="C68" s="3"/>
       <c r="D68" s="10"/>
-      <c r="E68" s="21" t="s">
+      <c r="E68" s="20" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1415,7 +1406,7 @@
       <c r="B69" s="2"/>
       <c r="C69" s="3"/>
       <c r="D69" s="10"/>
-      <c r="E69" s="21" t="s">
+      <c r="E69" s="20" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1424,7 +1415,7 @@
       <c r="B70" s="2"/>
       <c r="C70" s="3"/>
       <c r="D70" s="10"/>
-      <c r="E70" s="21" t="s">
+      <c r="E70" s="20" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1433,7 +1424,7 @@
       <c r="B71" s="2"/>
       <c r="C71" s="3"/>
       <c r="D71" s="10"/>
-      <c r="E71" s="21" t="s">
+      <c r="E71" s="20" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1442,7 +1433,7 @@
       <c r="B72" s="2"/>
       <c r="C72" s="3"/>
       <c r="D72" s="10"/>
-      <c r="E72" s="21" t="s">
+      <c r="E72" s="20" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1451,7 +1442,7 @@
       <c r="B73" s="2"/>
       <c r="C73" s="3"/>
       <c r="D73" s="10"/>
-      <c r="E73" s="21" t="s">
+      <c r="E73" s="20" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1460,7 +1451,7 @@
       <c r="B74" s="2"/>
       <c r="C74" s="3"/>
       <c r="D74" s="10"/>
-      <c r="E74" s="21" t="s">
+      <c r="E74" s="20" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1469,7 +1460,7 @@
       <c r="B75" s="2"/>
       <c r="C75" s="3"/>
       <c r="D75" s="10"/>
-      <c r="E75" s="21" t="s">
+      <c r="E75" s="20" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1478,7 +1469,7 @@
       <c r="B76" s="2"/>
       <c r="C76" s="3"/>
       <c r="D76" s="10"/>
-      <c r="E76" s="21" t="s">
+      <c r="E76" s="20" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1487,7 +1478,7 @@
       <c r="B77" s="2"/>
       <c r="C77" s="3"/>
       <c r="D77" s="10"/>
-      <c r="E77" s="21" t="s">
+      <c r="E77" s="20" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1496,7 +1487,7 @@
       <c r="B78" s="2"/>
       <c r="C78" s="3"/>
       <c r="D78" s="10"/>
-      <c r="E78" s="21" t="s">
+      <c r="E78" s="20" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1505,7 +1496,7 @@
       <c r="B79" s="2"/>
       <c r="C79" s="3"/>
       <c r="D79" s="10"/>
-      <c r="E79" s="21" t="s">
+      <c r="E79" s="20" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1514,7 +1505,7 @@
       <c r="B80" s="2"/>
       <c r="C80" s="3"/>
       <c r="D80" s="10"/>
-      <c r="E80" s="21" t="s">
+      <c r="E80" s="20" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1523,7 +1514,7 @@
       <c r="B81" s="2"/>
       <c r="C81" s="3"/>
       <c r="D81" s="10"/>
-      <c r="E81" s="21" t="s">
+      <c r="E81" s="20" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1532,7 +1523,7 @@
       <c r="B82" s="2"/>
       <c r="C82" s="3"/>
       <c r="D82" s="10"/>
-      <c r="E82" s="21" t="s">
+      <c r="E82" s="20" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1541,7 +1532,7 @@
       <c r="B83" s="2"/>
       <c r="C83" s="3"/>
       <c r="D83" s="10"/>
-      <c r="E83" s="21" t="s">
+      <c r="E83" s="20" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1550,7 +1541,7 @@
       <c r="B84" s="2"/>
       <c r="C84" s="3"/>
       <c r="D84" s="10"/>
-      <c r="E84" s="21" t="s">
+      <c r="E84" s="20" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1559,7 +1550,7 @@
       <c r="B85" s="2"/>
       <c r="C85" s="3"/>
       <c r="D85" s="10"/>
-      <c r="E85" s="21" t="s">
+      <c r="E85" s="20" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1568,7 +1559,7 @@
       <c r="B86" s="2"/>
       <c r="C86" s="3"/>
       <c r="D86" s="10"/>
-      <c r="E86" s="21" t="s">
+      <c r="E86" s="20" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1577,7 +1568,7 @@
       <c r="B87" s="2"/>
       <c r="C87" s="3"/>
       <c r="D87" s="10"/>
-      <c r="E87" s="21" t="s">
+      <c r="E87" s="20" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1586,7 +1577,7 @@
       <c r="B88" s="2"/>
       <c r="C88" s="3"/>
       <c r="D88" s="10"/>
-      <c r="E88" s="21" t="s">
+      <c r="E88" s="20" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1595,7 +1586,7 @@
       <c r="B89" s="2"/>
       <c r="C89" s="3"/>
       <c r="D89" s="10"/>
-      <c r="E89" s="21" t="s">
+      <c r="E89" s="20" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1604,7 +1595,7 @@
       <c r="B90" s="2"/>
       <c r="C90" s="3"/>
       <c r="D90" s="10"/>
-      <c r="E90" s="21" t="s">
+      <c r="E90" s="20" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1613,7 +1604,7 @@
       <c r="B91" s="2"/>
       <c r="C91" s="3"/>
       <c r="D91" s="10"/>
-      <c r="E91" s="21" t="s">
+      <c r="E91" s="20" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1622,7 +1613,7 @@
       <c r="B92" s="2"/>
       <c r="C92" s="3"/>
       <c r="D92" s="10"/>
-      <c r="E92" s="21" t="s">
+      <c r="E92" s="20" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1631,7 +1622,7 @@
       <c r="B93" s="2"/>
       <c r="C93" s="3"/>
       <c r="D93" s="10"/>
-      <c r="E93" s="21" t="s">
+      <c r="E93" s="20" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1640,7 +1631,7 @@
       <c r="B94" s="2"/>
       <c r="C94" s="3"/>
       <c r="D94" s="10"/>
-      <c r="E94" s="21" t="s">
+      <c r="E94" s="20" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1649,7 +1640,7 @@
       <c r="B95" s="2"/>
       <c r="C95" s="3"/>
       <c r="D95" s="10"/>
-      <c r="E95" s="21" t="s">
+      <c r="E95" s="20" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1658,7 +1649,7 @@
       <c r="B96" s="2"/>
       <c r="C96" s="3"/>
       <c r="D96" s="10"/>
-      <c r="E96" s="21" t="s">
+      <c r="E96" s="20" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1667,7 +1658,7 @@
       <c r="B97" s="2"/>
       <c r="C97" s="3"/>
       <c r="D97" s="10"/>
-      <c r="E97" s="21" t="s">
+      <c r="E97" s="20" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1676,7 +1667,7 @@
       <c r="B98" s="2"/>
       <c r="C98" s="3"/>
       <c r="D98" s="10"/>
-      <c r="E98" s="21" t="s">
+      <c r="E98" s="20" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1685,7 +1676,7 @@
       <c r="B99" s="2"/>
       <c r="C99" s="3"/>
       <c r="D99" s="10"/>
-      <c r="E99" s="21" t="s">
+      <c r="E99" s="20" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1694,7 +1685,7 @@
       <c r="B100" s="2"/>
       <c r="C100" s="3"/>
       <c r="D100" s="10"/>
-      <c r="E100" s="21" t="s">
+      <c r="E100" s="20" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
visualizacoes d eevolucao e bertopic inicial
</commit_message>
<xml_diff>
--- a/State of Art/Article KeyWords.xlsx
+++ b/State of Art/Article KeyWords.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\claud\OneDrive\Ambiente de Trabalho\tese\State of Art\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD9BDD65-4E5B-4391-8986-2511AC3AEFC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB146895-2A0D-49ED-886C-4D9B55926EFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{A4B60097-D1DB-47A4-812B-C06D94CFCCF5}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="54">
   <si>
     <t>Article</t>
   </si>
@@ -165,6 +165,41 @@
   </si>
   <si>
     <t>Dynamic Topic Quality, Temporal, Static Quality Score, coherence, diversity</t>
+  </si>
+  <si>
+    <t>https://people.eecs.berkeley.edu/~jfc/hcc/courseSP05/lecs/lec14/NMF03.pdf</t>
+  </si>
+  <si>
+    <t>Topic Modeling, Aviation Safety, Aviation
+Accident Reports, Machine Learning, LDA, NMF</t>
+  </si>
+  <si>
+    <t>Topic Modeling Analysis of Aviation Accident Reports: A Comparative Study between LDA and NMF Models</t>
+  </si>
+  <si>
+    <t>NMF vs LDA</t>
+  </si>
+  <si>
+    <t>NMF vs LDA vs BERTopic</t>
+  </si>
+  <si>
+    <t>Topic Modeling of the SrpELTeC Corpus:
+A Comparison of NMF, LDA, and BERTopic</t>
+  </si>
+  <si>
+    <t>topic modeling, LDA, NMF, BERTopic, SrpELTeC, computational literary studies</t>
+  </si>
+  <si>
+    <t>https://ieeexplore.ieee.org/stamp/stamp.jsp?tp=&amp;arnumber=10736093</t>
+  </si>
+  <si>
+    <t>https://www.jmlr.org/papers/volume3/blei03a/blei03a.pdf</t>
+  </si>
+  <si>
+    <t>LDA</t>
+  </si>
+  <si>
+    <t>Latent Dirichlet Allocation</t>
   </si>
 </sst>
 </file>
@@ -684,8 +719,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69BA454D-5C24-4BB5-BED8-A8161C909707}">
   <dimension ref="A1:E100"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -919,30 +954,54 @@
       </c>
     </row>
     <row r="14" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="1"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="9"/>
-      <c r="E14" s="19" t="s">
-        <v>7</v>
+      <c r="A14" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C14" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="D14" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="E14" s="4">
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="1"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="9"/>
-      <c r="E15" s="19" t="s">
-        <v>7</v>
+      <c r="A15" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C15" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="D15" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="E15" s="4">
+        <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="1"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="9"/>
-      <c r="E16" s="19" t="s">
-        <v>7</v>
+      <c r="A16" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D16" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="E16" s="4">
+        <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
@@ -1715,6 +1774,9 @@
     <hyperlink ref="D11" r:id="rId10" xr:uid="{659AF92B-426E-471F-93AC-013A888D85BB}"/>
     <hyperlink ref="D12" r:id="rId11" xr:uid="{6A54F949-D2DF-4217-BC1D-B27368D767E9}"/>
     <hyperlink ref="D13" r:id="rId12" xr:uid="{65E617D6-1EBA-40D5-A363-8BF7B8F48D03}"/>
+    <hyperlink ref="D14" r:id="rId13" xr:uid="{98FE1BA7-2A03-4FA8-B797-66B23314CAFA}"/>
+    <hyperlink ref="D15" r:id="rId14" xr:uid="{0D3114F6-E219-493A-A958-F25B12F3CDBE}"/>
+    <hyperlink ref="D16" r:id="rId15" xr:uid="{C7CD8C88-63A1-4DED-8248-8B2C8A48122B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>